<commit_message>
More questions for Driver added
</commit_message>
<xml_diff>
--- a/Data/user_data.xlsx
+++ b/Data/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Role</t>
+          <t>Question 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cargo</t>
+          <t>Question 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Car</t>
+          <t>Question 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Question 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Question 5</t>
         </is>
       </c>
     </row>
@@ -461,13 +471,105 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Водитель</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>Test user</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>55</v>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>volvo</t>
+          <t>Mitsubishi</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>moscow</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>396358609</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>oleg</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>44</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>mazda</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>rovno</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>396358610</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>55</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>toyota</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>wroclaw</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>396358608</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>test driver</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>logan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rostow</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed ReplyButton to InlineButton, added check algorithm in order to verity if user was registered
</commit_message>
<xml_diff>
--- a/Data/user_data.xlsx
+++ b/Data/user_data.xlsx
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -446,7 +446,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>user_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -474,7 +474,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>396358608</v>
+        <v>549874715</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -483,27 +483,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>Марина боровик</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>Бентли</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>Вроцлав</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -511,44 +511,34 @@
       <c r="A3" t="n">
         <v>396358608</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>396358608</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Брокер</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>396358608</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Брокер</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>396358608</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Брокер</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>396358608</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Брокер</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Водитель</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Illia</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fg</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ggg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added excel file cargo_data to store data about new cargo, also exdented Driver query to allow to choose cargo and assing it to specific driver
</commit_message>
<xml_diff>
--- a/Data/user_data.xlsx
+++ b/Data/user_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="11784" yWindow="2040" windowWidth="10248" windowHeight="9132" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="10488" yWindow="2136" windowWidth="10248" windowHeight="9132" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -469,8 +469,16 @@
       <c r="G1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Груз 1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Груз 2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -518,27 +526,37 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Illia</t>
+          <t>Илья</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ff</t>
+          <t>Вольво</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>fg</t>
+          <t>Вроцлав</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ggg</t>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Москва_Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Керчь_Новочеркасск</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
More emoji, user data display button function implemented
</commit_message>
<xml_diff>
--- a/Data/user_data.xlsx
+++ b/Data/user_data.xlsx
@@ -1,38 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\illia\GitProjects\telegrambotkirill\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0525B8-E789-45EF-9F8C-98A4078A198D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="10488" yWindow="2136" windowWidth="10248" windowHeight="9132" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="10488" yWindow="2136" windowWidth="10248" windowHeight="9132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Груз 1</t>
+  </si>
+  <si>
+    <t>Груз 2</t>
+  </si>
+  <si>
+    <t>Водитель</t>
+  </si>
+  <si>
+    <t>Марина боровик</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Бентли</t>
+  </si>
+  <si>
+    <t>Вроцлав</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Илья Пастушок</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Вольво</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,83 +118,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,134 +423,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:M3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M3" sqref="J3:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>user_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Role</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="1">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Груз 1</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Груз 2</t>
-        </is>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>549874715</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Водитель</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Марина боровик</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Бентли</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Вроцлав</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>396358608</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Водитель</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Илья</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Вольво</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Вроцлав</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Москва_Ростов-на-Дону</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Керчь_Новочеркасск</t>
-        </is>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Driver questions updated, broker role query updated
</commit_message>
<xml_diff>
--- a/Data/user_data.xlsx
+++ b/Data/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\illia\GitProjects\telegrambotkirill\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0943D6DA-72BD-41A8-8CA7-4CD45F7A0F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9260B62-5491-45E2-8013-B222A7F2E635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10488" yWindow="2136" windowWidth="10248" windowHeight="9132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>user_id</t>
   </si>
@@ -28,46 +28,40 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Груз 1</t>
-  </si>
-  <si>
-    <t>Груз 2</t>
-  </si>
-  <si>
-    <t>Водитель</t>
-  </si>
-  <si>
-    <t>Марина боровик</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Бентли</t>
-  </si>
-  <si>
-    <t>Вроцлав</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Илья</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>вольво</t>
-  </si>
-  <si>
-    <t>Ровно</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Брокер</t>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Телефон</t>
+  </si>
+  <si>
+    <t>Гос. Знак</t>
+  </si>
+  <si>
+    <t>Грузоподьемность</t>
+  </si>
+  <si>
+    <t>Измерения</t>
+  </si>
+  <si>
+    <t>Кузов</t>
+  </si>
+  <si>
+    <t>Город</t>
+  </si>
+  <si>
+    <t>Дистанция</t>
+  </si>
+  <si>
+    <t>ЮР. Статус</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Владение </t>
+  </si>
+  <si>
+    <t>Грузы</t>
+  </si>
+  <si>
+    <t>Тип загрузки</t>
   </si>
 </sst>
 </file>
@@ -96,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -119,13 +113,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -430,87 +438,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>549874715</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>396358608</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>